<commit_message>
Finished updates to the HTG for v1.5
</commit_message>
<xml_diff>
--- a/v1.5/Tools/OpenSAMM_Assessment_Toolbox_v1.5-Alpha.xlsx
+++ b/v1.5/Tools/OpenSAMM_Assessment_Toolbox_v1.5-Alpha.xlsx
@@ -12634,8 +12634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E342" sqref="E342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>